<commit_message>
update to normalisation spreadsheet
</commit_message>
<xml_diff>
--- a/normalization_spreadsheet.xlsx
+++ b/normalization_spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davideyre/Drive/academic/research/n_gonorrhoeae/mic_prediction_book_chapter/git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FDB37D45-7F94-F04F-8814-9E0F462699AC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{379B8277-774F-A04F-97D0-637442492279}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="50840" windowHeight="24100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,10 +444,10 @@
     </r>
   </si>
   <si>
-    <t>Manual normalization of libraries after PCR clean up in Nextera XT protocol to optimise cluster density</t>
-  </si>
-  <si>
     <t>This appendix is for multiplexing 48 samples using Nextera XT. However, it can be adjusted to the examined number of samples either by deleting rows or by copying and inserting additional rows. The formulae in Q9 and R9 also need to be adjusted to cover all samples.</t>
+  </si>
+  <si>
+    <t>Manual normalization of libraries after PCR clean up in Nextera XT protocol</t>
   </si>
 </sst>
 </file>
@@ -457,9 +457,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -711,112 +718,112 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1103,10 +1110,10 @@
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1155,7 +1162,7 @@
       <c r="A2" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="49"/>
+      <c r="B2" s="43"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="O3" s="4"/>
@@ -1164,8 +1171,8 @@
       <c r="A4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="49" t="s">
-        <v>109</v>
+      <c r="B4" s="43" t="s">
+        <v>108</v>
       </c>
       <c r="O4" s="4"/>
     </row>
@@ -1173,7 +1180,7 @@
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="44" t="s">
         <v>106</v>
       </c>
       <c r="O5" s="4"/>
@@ -1185,72 +1192,72 @@
       <c r="B6" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
       <c r="L6" s="60" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M6" s="60"/>
       <c r="N6" s="60"/>
       <c r="O6" s="60"/>
       <c r="P6" s="60"/>
-      <c r="Q6" s="61" t="s">
+      <c r="Q6" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="R6" s="61"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="61"/>
-      <c r="V6" s="61"/>
-      <c r="W6" s="61"/>
-      <c r="X6" s="61"/>
-      <c r="Y6" s="61"/>
-      <c r="Z6" s="62" t="s">
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
+      <c r="Z6" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="AA6" s="62"/>
-      <c r="AB6" s="62"/>
-      <c r="AC6" s="62"/>
-      <c r="AD6" s="62"/>
-      <c r="AE6" s="62"/>
-      <c r="AF6" s="62"/>
-      <c r="AG6" s="62"/>
+      <c r="AA6" s="56"/>
+      <c r="AB6" s="56"/>
+      <c r="AC6" s="56"/>
+      <c r="AD6" s="56"/>
+      <c r="AE6" s="56"/>
+      <c r="AF6" s="56"/>
+      <c r="AG6" s="56"/>
     </row>
     <row r="7" spans="1:33" ht="19" x14ac:dyDescent="0.25">
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="F7" s="46" t="s">
+      <c r="D7" s="57"/>
+      <c r="F7" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="46"/>
-      <c r="J7" s="51" t="s">
+      <c r="G7" s="57"/>
+      <c r="J7" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="51"/>
-      <c r="V7" s="48" t="s">
+      <c r="K7" s="58"/>
+      <c r="V7" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="W7" s="48"/>
-      <c r="Z7" s="43" t="s">
+      <c r="W7" s="61"/>
+      <c r="Z7" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="AA7" s="43"/>
-      <c r="AE7" s="43" t="s">
+      <c r="AA7" s="53"/>
+      <c r="AE7" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="AF7" s="43"/>
-      <c r="AG7" s="43"/>
+      <c r="AF7" s="53"/>
+      <c r="AG7" s="53"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -1280,10 +1287,10 @@
       <c r="I8" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="J8" s="52" t="s">
+      <c r="J8" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="K8" s="46" t="s">
         <v>57</v>
       </c>
       <c r="L8" s="6" t="s">
@@ -1380,11 +1387,11 @@
         <f>(H9*100)/0.2</f>
         <v>0</v>
       </c>
-      <c r="J9" s="54">
+      <c r="J9" s="47">
         <f>I9-100</f>
         <v>-100</v>
       </c>
-      <c r="K9" s="55"/>
+      <c r="K9" s="48"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="9" t="e">
@@ -1482,11 +1489,11 @@
         <f t="shared" ref="I10:I56" si="3">(H10*100)/0.2</f>
         <v>0</v>
       </c>
-      <c r="J10" s="54">
+      <c r="J10" s="47">
         <f t="shared" ref="J10:J54" si="4">I10-100</f>
         <v>-100</v>
       </c>
-      <c r="K10" s="55"/>
+      <c r="K10" s="48"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="9" t="e">
@@ -1530,11 +1537,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J11" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K11" s="55"/>
+      <c r="J11" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K11" s="48"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="9" t="e">
@@ -1576,11 +1583,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J12" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K12" s="55"/>
+      <c r="J12" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K12" s="48"/>
       <c r="L12" s="37"/>
       <c r="M12" s="11"/>
       <c r="N12" s="9" t="e">
@@ -1623,11 +1630,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J13" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K13" s="55"/>
+      <c r="J13" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K13" s="48"/>
       <c r="L13" s="37"/>
       <c r="M13" s="11"/>
       <c r="N13" s="9" t="e">
@@ -1671,11 +1678,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J14" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K14" s="55"/>
+      <c r="J14" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K14" s="48"/>
       <c r="L14" s="37"/>
       <c r="M14" s="11"/>
       <c r="N14" s="9" t="e">
@@ -1719,11 +1726,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J15" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K15" s="55"/>
+      <c r="J15" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K15" s="48"/>
       <c r="L15" s="37"/>
       <c r="M15" s="11"/>
       <c r="N15" s="9" t="e">
@@ -1768,11 +1775,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J16" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K16" s="55"/>
+      <c r="J16" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K16" s="48"/>
       <c r="L16" s="37"/>
       <c r="M16" s="11"/>
       <c r="N16" s="9" t="e">
@@ -1815,11 +1822,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J17" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K17" s="55"/>
+      <c r="J17" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K17" s="48"/>
       <c r="L17" s="37"/>
       <c r="M17" s="11"/>
       <c r="N17" s="9" t="e">
@@ -1863,11 +1870,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J18" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K18" s="55"/>
+      <c r="J18" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K18" s="48"/>
       <c r="L18" s="37"/>
       <c r="M18" s="11"/>
       <c r="N18" s="9" t="e">
@@ -1911,11 +1918,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J19" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K19" s="55"/>
+      <c r="J19" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K19" s="48"/>
       <c r="L19" s="37"/>
       <c r="M19" s="11"/>
       <c r="N19" s="9" t="e">
@@ -1960,11 +1967,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J20" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K20" s="55"/>
+      <c r="J20" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K20" s="48"/>
       <c r="L20" s="37"/>
       <c r="M20" s="11"/>
       <c r="N20" s="9" t="e">
@@ -2007,11 +2014,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K21" s="55"/>
+      <c r="J21" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K21" s="48"/>
       <c r="L21" s="37"/>
       <c r="M21" s="11"/>
       <c r="N21" s="9" t="e">
@@ -2055,11 +2062,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J22" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K22" s="55"/>
+      <c r="J22" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K22" s="48"/>
       <c r="L22" s="37"/>
       <c r="M22" s="11"/>
       <c r="N22" s="9" t="e">
@@ -2103,11 +2110,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J23" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K23" s="55"/>
+      <c r="J23" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K23" s="48"/>
       <c r="L23" s="37"/>
       <c r="M23" s="11"/>
       <c r="N23" s="9" t="e">
@@ -2152,11 +2159,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K24" s="55"/>
+      <c r="J24" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K24" s="48"/>
       <c r="L24" s="37"/>
       <c r="M24" s="11"/>
       <c r="N24" s="9" t="e">
@@ -2199,11 +2206,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J25" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K25" s="55"/>
+      <c r="J25" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K25" s="48"/>
       <c r="L25" s="37"/>
       <c r="M25" s="11"/>
       <c r="N25" s="9" t="e">
@@ -2246,11 +2253,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J26" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K26" s="55"/>
+      <c r="J26" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K26" s="48"/>
       <c r="L26" s="37"/>
       <c r="M26" s="11"/>
       <c r="N26" s="9" t="e">
@@ -2294,11 +2301,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J27" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K27" s="55"/>
+      <c r="J27" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K27" s="48"/>
       <c r="L27" s="37"/>
       <c r="M27" s="11"/>
       <c r="N27" s="9" t="e">
@@ -2342,11 +2349,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J28" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K28" s="55"/>
+      <c r="J28" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K28" s="48"/>
       <c r="L28" s="37"/>
       <c r="M28" s="11"/>
       <c r="N28" s="9" t="e">
@@ -2390,11 +2397,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J29" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K29" s="55"/>
+      <c r="J29" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K29" s="48"/>
       <c r="L29" s="37"/>
       <c r="M29" s="11"/>
       <c r="N29" s="9" t="e">
@@ -2436,11 +2443,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J30" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K30" s="55"/>
+      <c r="J30" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K30" s="48"/>
       <c r="L30" s="37"/>
       <c r="M30" s="11"/>
       <c r="N30" s="9" t="e">
@@ -2487,11 +2494,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J31" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K31" s="55"/>
+      <c r="J31" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K31" s="48"/>
       <c r="L31" s="37"/>
       <c r="M31" s="11"/>
       <c r="N31" s="9" t="e">
@@ -2538,11 +2545,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J32" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K32" s="55"/>
+      <c r="J32" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K32" s="48"/>
       <c r="L32" s="37"/>
       <c r="M32" s="11"/>
       <c r="N32" s="9" t="e">
@@ -2589,11 +2596,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J33" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K33" s="55"/>
+      <c r="J33" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K33" s="48"/>
       <c r="L33" s="37"/>
       <c r="M33" s="11"/>
       <c r="N33" s="9" t="e">
@@ -2635,11 +2642,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J34" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K34" s="55"/>
+      <c r="J34" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K34" s="48"/>
       <c r="L34" s="37"/>
       <c r="M34" s="11"/>
       <c r="N34" s="9" t="e">
@@ -2686,11 +2693,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J35" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K35" s="55"/>
+      <c r="J35" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K35" s="48"/>
       <c r="L35" s="37"/>
       <c r="M35" s="11"/>
       <c r="N35" s="9" t="e">
@@ -2732,11 +2739,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J36" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K36" s="55"/>
+      <c r="J36" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K36" s="48"/>
       <c r="L36" s="37"/>
       <c r="M36" s="11"/>
       <c r="N36" s="9" t="e">
@@ -2783,11 +2790,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J37" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K37" s="55"/>
+      <c r="J37" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K37" s="48"/>
       <c r="L37" s="37"/>
       <c r="M37" s="11"/>
       <c r="N37" s="9" t="e">
@@ -2834,11 +2841,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J38" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K38" s="55"/>
+      <c r="J38" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K38" s="48"/>
       <c r="L38" s="37"/>
       <c r="M38" s="11"/>
       <c r="N38" s="9" t="e">
@@ -2885,11 +2892,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J39" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K39" s="55"/>
+      <c r="J39" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K39" s="48"/>
       <c r="L39" s="37"/>
       <c r="M39" s="11"/>
       <c r="N39" s="9" t="e">
@@ -2936,11 +2943,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J40" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K40" s="55"/>
+      <c r="J40" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K40" s="48"/>
       <c r="L40" s="37"/>
       <c r="M40" s="11"/>
       <c r="N40" s="9" t="e">
@@ -2987,11 +2994,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J41" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K41" s="55"/>
+      <c r="J41" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K41" s="48"/>
       <c r="L41" s="37"/>
       <c r="M41" s="11"/>
       <c r="N41" s="9" t="e">
@@ -3033,11 +3040,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J42" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K42" s="55"/>
+      <c r="J42" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K42" s="48"/>
       <c r="L42" s="37"/>
       <c r="M42" s="11"/>
       <c r="N42" s="9" t="e">
@@ -3079,11 +3086,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J43" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K43" s="55"/>
+      <c r="J43" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K43" s="48"/>
       <c r="L43" s="37"/>
       <c r="M43" s="11"/>
       <c r="N43" s="9" t="e">
@@ -3130,11 +3137,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J44" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K44" s="55"/>
+      <c r="J44" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K44" s="48"/>
       <c r="L44" s="37"/>
       <c r="M44" s="11"/>
       <c r="N44" s="9" t="e">
@@ -3181,11 +3188,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J45" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K45" s="55"/>
+      <c r="J45" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K45" s="48"/>
       <c r="L45" s="37"/>
       <c r="M45" s="11"/>
       <c r="N45" s="9" t="e">
@@ -3232,11 +3239,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J46" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K46" s="55"/>
+      <c r="J46" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K46" s="48"/>
       <c r="L46" s="37"/>
       <c r="M46" s="11"/>
       <c r="N46" s="9" t="e">
@@ -3278,11 +3285,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J47" s="56">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K47" s="57"/>
+      <c r="J47" s="49">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K47" s="50"/>
       <c r="L47" s="37"/>
       <c r="M47" s="11"/>
       <c r="N47" s="31" t="e">
@@ -3329,11 +3336,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J48" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K48" s="55"/>
+      <c r="J48" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K48" s="48"/>
       <c r="L48" s="37"/>
       <c r="M48" s="11"/>
       <c r="N48" s="9" t="e">
@@ -3380,11 +3387,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J49" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K49" s="55"/>
+      <c r="J49" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K49" s="48"/>
       <c r="L49" s="37"/>
       <c r="M49" s="11"/>
       <c r="N49" s="9" t="e">
@@ -3426,11 +3433,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J50" s="58">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K50" s="59"/>
+      <c r="J50" s="51">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K50" s="52"/>
       <c r="L50" s="37"/>
       <c r="M50" s="11"/>
       <c r="N50" s="18" t="e">
@@ -3472,11 +3479,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J51" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K51" s="55"/>
+      <c r="J51" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K51" s="48"/>
       <c r="L51" s="37"/>
       <c r="M51" s="11"/>
       <c r="N51" s="9" t="e">
@@ -3518,11 +3525,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J52" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K52" s="55"/>
+      <c r="J52" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K52" s="48"/>
       <c r="L52" s="37"/>
       <c r="M52" s="11"/>
       <c r="N52" s="9" t="e">
@@ -3564,11 +3571,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J53" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K53" s="55"/>
+      <c r="J53" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K53" s="48"/>
       <c r="L53" s="37"/>
       <c r="M53" s="11"/>
       <c r="N53" s="9" t="e">
@@ -3610,11 +3617,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J54" s="54">
-        <f t="shared" si="4"/>
-        <v>-100</v>
-      </c>
-      <c r="K54" s="55"/>
+      <c r="J54" s="47">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K54" s="48"/>
       <c r="L54" s="37"/>
       <c r="M54" s="11"/>
       <c r="N54" s="9" t="e">
@@ -3656,11 +3663,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J55" s="54">
+      <c r="J55" s="47">
         <f t="shared" ref="J55:J56" si="9">I55-100</f>
         <v>-100</v>
       </c>
-      <c r="K55" s="55"/>
+      <c r="K55" s="48"/>
       <c r="L55" s="37"/>
       <c r="M55" s="11"/>
       <c r="N55" s="9" t="e">
@@ -3702,11 +3709,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J56" s="54">
+      <c r="J56" s="47">
         <f t="shared" si="9"/>
         <v>-100</v>
       </c>
-      <c r="K56" s="55"/>
+      <c r="K56" s="48"/>
       <c r="L56" s="37"/>
       <c r="M56" s="11"/>
       <c r="N56" s="9" t="e">
@@ -3752,20 +3759,20 @@
       <c r="X57" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="Z57" s="44" t="s">
+      <c r="Z57" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="AA57" s="45"/>
+      <c r="AA57" s="55"/>
       <c r="AD57" s="21" t="s">
         <v>73</v>
       </c>
       <c r="AE57" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="AF57" s="44" t="s">
+      <c r="AF57" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="AG57" s="45"/>
+      <c r="AG57" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>